<commit_message>
Adding in support for LiquidCool Node 1
</commit_message>
<xml_diff>
--- a/projects/lhs_discrete_continuous_example.xlsx
+++ b/projects/lhs_discrete_continuous_example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="51200" windowHeight="28260" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -3997,10 +3997,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1497">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5800,8 +5800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6078,14 +6078,14 @@
       </c>
       <c r="B23" s="17">
         <f>IF(D23&lt;&gt;"",D23,IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B19,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B19,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="C23" s="24" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B19,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B19,Lookups!$A$21:$A$27,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D23" s="26">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="E23" s="22"/>
     </row>
@@ -6335,7 +6335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
@@ -6393,14 +6393,14 @@
       <c r="R1" s="30"/>
       <c r="S1" s="27"/>
       <c r="T1" s="27"/>
-      <c r="U1" s="47" t="s">
+      <c r="U1" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
     </row>
     <row r="2" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A2" s="31" t="s">
@@ -7765,42 +7765,42 @@
       <c r="Z34" s="36"/>
     </row>
     <row r="35" spans="1:26">
-      <c r="A35" s="48"/>
-      <c r="B35" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48" t="s">
+      <c r="A35" s="47"/>
+      <c r="B35" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47" t="s">
         <v>736</v>
       </c>
-      <c r="E35" s="48" t="s">
+      <c r="E35" s="47" t="s">
         <v>734</v>
       </c>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48" t="s">
+      <c r="F35" s="47"/>
+      <c r="G35" s="47" t="s">
         <v>735</v>
       </c>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48" t="b">
+      <c r="H35" s="47"/>
+      <c r="I35" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="48"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="48"/>
-      <c r="O35" s="48"/>
-      <c r="P35" s="48"/>
-      <c r="Q35" s="48"/>
-      <c r="R35" s="48"/>
-      <c r="S35" s="48"/>
-      <c r="T35" s="48"/>
-      <c r="U35" s="48"/>
-      <c r="V35" s="48"/>
-      <c r="W35" s="48"/>
-      <c r="X35" s="48"/>
-      <c r="Y35" s="48"/>
-      <c r="Z35" s="48"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="47"/>
+      <c r="Q35" s="47"/>
+      <c r="R35" s="47"/>
+      <c r="S35" s="47"/>
+      <c r="T35" s="47"/>
+      <c r="U35" s="47"/>
+      <c r="V35" s="47"/>
+      <c r="W35" s="47"/>
+      <c r="X35" s="47"/>
+      <c r="Y35" s="47"/>
+      <c r="Z35" s="47"/>
     </row>
     <row r="36" spans="1:26">
       <c r="A36" s="39"/>

</xml_diff>

<commit_message>
CLI fix, thanks to Scott for noticing!
</commit_message>
<xml_diff>
--- a/projects/lhs_discrete_continuous_example.xlsx
+++ b/projects/lhs_discrete_continuous_example.xlsx
@@ -6078,14 +6078,14 @@
       </c>
       <c r="B23" s="17">
         <f>IF(D23&lt;&gt;"",D23,IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B19,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B19,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="C23" s="24" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B19,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B19,Lookups!$A$21:$A$27,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D23" s="26">
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="E23" s="22"/>
     </row>

</xml_diff>